<commit_message>
Workshop Plenaries and html file name changed
</commit_message>
<xml_diff>
--- a/polls/IROS2020_onDemand.xlsx
+++ b/polls/IROS2020_onDemand.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akdba\Desktop\mysite\polls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FE2038-87D9-4F96-8498-6B0B6ADB3F5E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2777B6-8313-4A4A-89E4-CD253082262D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -1003,15 +1003,15 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="41.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1132,10 +1132,10 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1235,10 +1235,10 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="53.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>